<commit_message>
add results on top5 apps explorations (for PhD)
</commit_message>
<xml_diff>
--- a/resources/top_apps/top5_apks_metadata/apps_metadata.xlsx
+++ b/resources/top_apps/top5_apks_metadata/apps_metadata.xlsx
@@ -22,8 +22,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="H16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The pop-up:
+APUS
+It seems that your APUS Launcher is corrupted. Would you like to install it again from Google Play?
+OK Cancel</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="180">
   <si>
     <t xml:space="preserve">/jacobs/APKs/an/anim/animaonl/animaonline.android.wikiexplorer/1.5.5/animaonline.android.wikiexplorer.apk            </t>
   </si>
@@ -512,13 +549,64 @@
   </si>
   <si>
     <t>Duplicates happen because the apps are present in multiple categories.</t>
+  </si>
+  <si>
+    <t>com.apusapps.launcher_v1.4.0.apk</t>
+  </si>
+  <si>
+    <t>OK apps</t>
+  </si>
+  <si>
+    <t>de.mcdonalds.mcdonaldsinfoapp_v1.4.0.1.apk</t>
+  </si>
+  <si>
+    <t>Pre-filtered</t>
+  </si>
+  <si>
+    <t>Cannot even start exploration</t>
+  </si>
+  <si>
+    <t>Terminates early: no meaningful exploration possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waiting for GUI stabilization succeeds in spite of GUI still loading. Longer delays would make the app load properly. </t>
+  </si>
+  <si>
+    <t>Solutions:</t>
+  </si>
+  <si>
+    <t>Explore by launching both activties.</t>
+  </si>
+  <si>
+    <t>Somehow find the base app extended by these and explore it, diffing the behavior change.</t>
+  </si>
+  <si>
+    <t>As with "Cannot launch: no activity or app icon"</t>
+  </si>
+  <si>
+    <t>Avoid inlining by using Boxify or instrumenting OS.</t>
+  </si>
+  <si>
+    <t>Try again after a delay. Do it only if initial reset had actionable widgets.</t>
+  </si>
+  <si>
+    <t>No actionable widgets after second reset due to delays</t>
+  </si>
+  <si>
+    <t>No actionable widgets after second reset due to delays.</t>
+  </si>
+  <si>
+    <t>Integrity check detects inlining: everything blacklisted.</t>
+  </si>
+  <si>
+    <t>Usually manifests by the affected app displaying a pop-up dialog box on launching main activity informing the app is corrupted. Manually confirmed that non-inlined apps work. After pressing all pop-up box widgets they all become blacklisted and exploration terminates.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,14 +622,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,6 +678,23 @@
         <fgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -574,22 +705,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
+    <cellStyle name="60% - Accent6" xfId="5" builtinId="52"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -615,6 +761,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -922,25 +1073,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="10.36328125" customWidth="1"/>
     <col min="3" max="3" width="10.08984375" customWidth="1"/>
     <col min="5" max="5" width="11.453125" customWidth="1"/>
     <col min="6" max="6" width="57.81640625" customWidth="1"/>
-    <col min="7" max="7" width="34.08984375" customWidth="1"/>
+    <col min="7" max="7" width="46.81640625" customWidth="1"/>
     <col min="8" max="8" width="59" customWidth="1"/>
+    <col min="10" max="10" width="43.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>145</v>
       </c>
@@ -959,8 +1111,11 @@
       <c r="H1" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J1" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -982,18 +1137,11 @@
       <c r="H2" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <f>C2-B3</f>
-        <v>126</v>
-      </c>
+      <c r="J2" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="E3" s="1" t="s">
         <v>142</v>
       </c>
@@ -1007,16 +1155,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <f>C3-B4</f>
-        <v>125</v>
+    <row r="4" spans="1:10">
+      <c r="A4" s="10" t="s">
+        <v>166</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>143</v>
@@ -1031,146 +1172,285 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>C2-B5</f>
+        <v>126</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="E6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f>C5-B8</f>
+        <v>125</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B5">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C5">
-        <f>C4-B5</f>
+      <c r="C9">
+        <f>C8-B9</f>
         <v>124</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F9" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <f>C9-B10</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>C10-B11</f>
+        <v>119</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="E12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f>C11-B14</f>
+        <v>118</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f>C14-B15</f>
+        <v>117</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="10"/>
+      <c r="E16" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <f>C5-B6</f>
-        <v>120</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <f>C6-B7</f>
-        <v>119</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F8" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E10" s="1" t="s">
+      <c r="F16" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="F17" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="F18" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="F19" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="E21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E11" s="1" t="s">
+      <c r="F21" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="E22" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E12" s="1" t="s">
+    </row>
+    <row r="23" spans="2:6">
+      <c r="E23" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E13" s="1" t="s">
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="9"/>
+      <c r="C24" s="8"/>
+      <c r="E24" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E14" s="1" t="s">
+      <c r="F24" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="4"/>
+      <c r="E25" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="E26" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F15" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F16" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F17" s="3" t="s">
-        <v>154</v>
+      <c r="F26" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="F14:F17">
+  <sortState ref="F16:F19">
     <sortCondition ref="F17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1180,634 +1460,634 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1">
       <c r="A68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1">
       <c r="A71" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1">
       <c r="A72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1">
       <c r="A73" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1">
       <c r="A74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1">
       <c r="A75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1">
       <c r="A76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1">
       <c r="A77" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1">
       <c r="A78" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1">
       <c r="A79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1">
       <c r="A80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1">
       <c r="A81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1">
       <c r="A83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1">
       <c r="A84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1">
       <c r="A85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1">
       <c r="A86" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1">
       <c r="A87" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1">
       <c r="A88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1">
       <c r="A89" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1">
       <c r="A90" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1">
       <c r="A91" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1">
       <c r="A92" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1">
       <c r="A93" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1">
       <c r="A94" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1">
       <c r="A95" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1">
       <c r="A96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1">
       <c r="A98" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1">
       <c r="A99" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1">
       <c r="A101" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1">
       <c r="A102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1">
       <c r="A103" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1">
       <c r="A104" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1">
       <c r="A105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1">
       <c r="A106" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1">
       <c r="A107" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1">
       <c r="A108" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1">
       <c r="A109" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1">
       <c r="A110" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1">
       <c r="A111" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1">
       <c r="A112" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1">
       <c r="A113" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1">
       <c r="A114" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1">
       <c r="A115" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1">
       <c r="A116" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1">
       <c r="A117" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1">
       <c r="A118" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1">
       <c r="A119" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1">
       <c r="A120" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1">
       <c r="A121" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1">
       <c r="A122" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1">
       <c r="A123" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1">
       <c r="A124" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1">
       <c r="A125" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1">
       <c r="A126" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1">
       <c r="A127" t="s">
         <v>125</v>
       </c>

</xml_diff>

<commit_message>
update apps metadata (for PhD)
</commit_message>
<xml_diff>
--- a/resources/top_apps/top5_apks_metadata/apps_metadata.xlsx
+++ b/resources/top_apps/top5_apks_metadata/apps_metadata.xlsx
@@ -10,7 +10,7 @@
     <sheet name="apps_metadata" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">apps_metadata!$A$1:$E$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">apps_metadata!$A$1:$I$23</definedName>
   </definedNames>
   <calcPr calcId="171027" refMode="R1C1"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
   <si>
     <t xml:space="preserve">com.google.android.keep_v2.3.02.apk            </t>
   </si>
@@ -177,9 +177,6 @@
     <t>DM: Avoid inlining by using Boxify or instrumenting OS.</t>
   </si>
   <si>
-    <t>DM: Wait longer after app launch before checking for actionable widgets. Either for all apps or only for this one. Possibly do multiple checks, proceeding if app displays something already on first check, and giving up only when the last one fails.</t>
-  </si>
-  <si>
     <t>DM: Try again after a delay. Do it only if initial reset had actionable widgets.</t>
   </si>
   <si>
@@ -217,6 +214,102 @@
   </si>
   <si>
     <t>Processed:</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Widgets</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Live Wallpaper</t>
+  </si>
+  <si>
+    <t>Libraries &amp; Demo</t>
+  </si>
+  <si>
+    <t>Health &amp; Fitness</t>
+  </si>
+  <si>
+    <t>Personalization</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Media &amp; Video</t>
+  </si>
+  <si>
+    <t>Lifestyle</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>Processed top1:</t>
+  </si>
+  <si>
+    <t>Total top 1 apps:</t>
+  </si>
+  <si>
+    <t>Remaining to process top1:</t>
+  </si>
+  <si>
+    <t>Top1</t>
+  </si>
+  <si>
+    <t>com.facebook.katana_v28.0.0.20.16.apk</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>DM: Wait longer after app launch  (cfg.launchActivityDelay) before checking for actionable widgets. Either for all apps or only for this one. Possibly do multiple checks, proceeding if app displays something already on first check, and giving up only when the last one fails.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM: Wait longer (20 sec is not enough for cfg.launchActivityDelay) after app launch before checking for actionable widgets. Either for all apps or only for this one. Possibly do multiple checks, proceeding if app displays something already on first check, and giving up only when the last one fails. </t>
+  </si>
+  <si>
+    <t>com.infraware.office.link_v6.0.9.apk</t>
+  </si>
+  <si>
+    <t>03 Terminates on launch: quits to home screen.</t>
+  </si>
+  <si>
+    <t>Displays white screen for a moment, then just quits to home or apps screen.</t>
+  </si>
+  <si>
+    <t>App is defective. Logcat shows that ActivityManager reports the app process died. There are no exceptions thrown from the app. It happens also on the original, non-inlined app.</t>
+  </si>
+  <si>
+    <t>com.runtastic.android_v5.2.1.apk</t>
+  </si>
+  <si>
+    <t>The XML window hierarchy has no clickable widgets, just a widget with "SWIPE" label.</t>
+  </si>
+  <si>
+    <t>DroidMate doesn't support swipes. The only actionable widget is for swiping and it doesn't have the attributes that DroidMate considers as making a widget actionable.</t>
+  </si>
+  <si>
+    <t>DM: add ability to conduct swipes + add some GUI XML dump heuristic to recognize which widgets can be swiped and/or add static analysis of bytecode to find appropriate swip handlers attached to GUI widgets.</t>
   </si>
 </sst>
 </file>
@@ -304,7 +397,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -313,6 +406,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -638,378 +749,697 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="57.81640625" customWidth="1"/>
-    <col min="2" max="2" width="52.26953125" customWidth="1"/>
-    <col min="3" max="3" width="49.6328125" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" customWidth="1"/>
-    <col min="5" max="5" width="59.7265625" customWidth="1"/>
-    <col min="6" max="6" width="43.7265625" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="7.08984375" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="52.26953125" customWidth="1"/>
+    <col min="7" max="7" width="49.6328125" customWidth="1"/>
+    <col min="8" max="8" width="56.453125" customWidth="1"/>
+    <col min="9" max="9" width="59.7265625" customWidth="1"/>
+    <col min="10" max="10" width="43.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9">
+        <v>41927</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>41936</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>41893</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>41870</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9">
+        <v>41853</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="12">
+        <v>41881</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12">
+        <v>42069</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12">
+        <v>41885</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12">
+        <v>42060</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12">
+        <v>41937</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="12">
+        <v>41882</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12">
+        <v>41687</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1</v>
+      </c>
+      <c r="D14" s="12">
+        <v>42051</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="10">
+        <v>2</v>
+      </c>
+      <c r="D15" s="9">
+        <v>41937</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="10">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9">
+        <v>41922</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2</v>
+      </c>
+      <c r="D17" s="9">
+        <v>41887</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2</v>
+      </c>
+      <c r="D18" s="9">
+        <v>42045</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="10">
+        <v>2</v>
+      </c>
+      <c r="D19" s="9">
+        <v>41852</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2</v>
+      </c>
+      <c r="D20" s="12">
+        <v>41721</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="10">
+        <v>2</v>
+      </c>
+      <c r="D21" s="9">
+        <v>41897</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="D22" s="9">
+        <v>41853</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="G22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="I22" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="10">
+        <v>3</v>
+      </c>
+      <c r="D23" s="9">
+        <v>41888</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27">
+        <f>SUM(E2:E23)</f>
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28">
+        <f>B26-B27</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31">
+        <f>ROWS(F2:F23)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>62</v>
       </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24">
-        <f>ROWS(B2:B20)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25">
-        <f>B23-B24</f>
-        <v>111</v>
+      <c r="B32">
+        <f>B30-B31</f>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E20">
-    <sortState ref="A2:E20">
-      <sortCondition ref="B1:B20"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update apps_metadata.xlsx -- DONE!
</commit_message>
<xml_diff>
--- a/resources/top_apps/top5_apks_metadata/apps_metadata.xlsx
+++ b/resources/top_apps/top5_apks_metadata/apps_metadata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="148">
   <si>
     <t xml:space="preserve">com.google.android.keep_v2.3.02.apk            </t>
   </si>
@@ -354,9 +354,6 @@
     <t>Books &amp; Reference</t>
   </si>
   <si>
-    <t>Note: app is in top1 if it is in C:\my\local\repos\sechair\droidmate-private\resources\top_apps\top5_apks_metadata\130app_entries_metadata.txt</t>
-  </si>
-  <si>
     <t>arlind.Shqip_v2.0.apk</t>
   </si>
   <si>
@@ -450,10 +447,25 @@
     <t>Finance</t>
   </si>
   <si>
-    <t>After it loads a popup "Get free gold coins for every push notification" with "OK" that is never clicked. Instead DM seems to click some invisible things.</t>
-  </si>
-  <si>
     <t>Weather</t>
+  </si>
+  <si>
+    <t>DM: Add heuristics to recognize popup boxes / "OK" buttons even if not marked as clickable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The popup box "OK" button is not marked as clickable, even though it is a TextView with res id com.outfit7.talkingangelafree:id/push_button and within current view bounds. </t>
+  </si>
+  <si>
+    <t>After it loads a popup "Get free gold coins for every push notification" with "OK" that is never clicked. Instead DM clicks on 3 buttons, stuck in same widget context, that cannot be manually inspected due to the popup box. Instead of randomizing clickin on the "OK" DM clicks on the "com.outfit7.talkingangelafree:id/topSoftViewPlaceholder" which is an ancestor of the dialog box whose area is almost the entire screen. Because OK button is not centered, it misses it.</t>
+  </si>
+  <si>
+    <t>Note: core feature not supported: text input for searching city</t>
+  </si>
+  <si>
+    <t>Note: core feature not supported: text input for setting from/to</t>
+  </si>
+  <si>
+    <t>Note: app is in top1 if it is listed in C:\my\local\repos\sechair\droidmate-private\resources\top_apps\top5_apks_metadata\130app_entries_metadata.txt</t>
   </si>
 </sst>
 </file>
@@ -486,7 +498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -540,8 +552,31 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -549,14 +584,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -585,22 +639,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="4" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="8">
+    <cellStyle name="20% - Accent3" xfId="5" builtinId="38"/>
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
+    <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
+    <cellStyle name="40% - Accent5" xfId="7" builtinId="47"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -922,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -981,7 +1046,7 @@
       <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <v>41927</v>
       </c>
       <c r="E2" s="11"/>
@@ -1005,7 +1070,7 @@
       <c r="C3" s="9">
         <v>2</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>41937</v>
       </c>
       <c r="E3" s="11"/>
@@ -1029,7 +1094,7 @@
       <c r="C4" s="9">
         <v>2</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>41922</v>
       </c>
       <c r="E4" s="11"/>
@@ -1053,7 +1118,7 @@
       <c r="C5" s="8">
         <v>2</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>41887</v>
       </c>
       <c r="E5" s="11"/>
@@ -1077,7 +1142,7 @@
       <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>41936</v>
       </c>
       <c r="E6" s="11"/>
@@ -1104,7 +1169,7 @@
       <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>41893</v>
       </c>
       <c r="E7" s="11">
@@ -1133,7 +1198,7 @@
       <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>41870</v>
       </c>
       <c r="E8" s="11"/>
@@ -1160,7 +1225,7 @@
       <c r="C9" s="9">
         <v>1</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>41853</v>
       </c>
       <c r="E9" s="11"/>
@@ -1187,7 +1252,7 @@
       <c r="C10" s="9">
         <v>2</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>42045</v>
       </c>
       <c r="E10" s="11"/>
@@ -1214,7 +1279,7 @@
       <c r="C11" s="9">
         <v>2</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>41852</v>
       </c>
       <c r="E11" s="11"/>
@@ -1241,7 +1306,7 @@
       <c r="C12" s="9">
         <v>3</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>41853</v>
       </c>
       <c r="E12" s="11"/>
@@ -1268,7 +1333,7 @@
       <c r="C13" s="8">
         <v>1</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>41881</v>
       </c>
       <c r="E13" s="11">
@@ -1297,7 +1362,7 @@
       <c r="C14" s="8">
         <v>1</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>42069</v>
       </c>
       <c r="E14" s="11">
@@ -1326,7 +1391,7 @@
       <c r="C15" s="8">
         <v>1</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <v>41885</v>
       </c>
       <c r="E15" s="11">
@@ -1355,7 +1420,7 @@
       <c r="C16" s="8">
         <v>2</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="17">
         <v>41721</v>
       </c>
       <c r="E16" s="11"/>
@@ -1382,7 +1447,7 @@
       <c r="C17" s="8">
         <v>1</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="17">
         <v>42060</v>
       </c>
       <c r="E17" s="11">
@@ -1411,7 +1476,7 @@
       <c r="C18" s="9">
         <v>2</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <v>41897</v>
       </c>
       <c r="E18" s="11"/>
@@ -1438,7 +1503,7 @@
       <c r="C19" s="8">
         <v>1</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="17">
         <v>41937</v>
       </c>
       <c r="E19" s="11"/>
@@ -1465,7 +1530,7 @@
       <c r="C20" s="9">
         <v>3</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>41888</v>
       </c>
       <c r="E20" s="11"/>
@@ -1492,7 +1557,7 @@
       <c r="C21" s="8">
         <v>1</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="17">
         <v>41882</v>
       </c>
       <c r="E21" s="11"/>
@@ -1519,7 +1584,7 @@
       <c r="C22" s="8">
         <v>1</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <v>41687</v>
       </c>
       <c r="E22" s="11"/>
@@ -1546,7 +1611,7 @@
       <c r="C23" s="8">
         <v>1</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="17">
         <v>41886</v>
       </c>
       <c r="E23" s="11">
@@ -1575,7 +1640,7 @@
       <c r="C24" s="8">
         <v>1</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="17">
         <v>41717</v>
       </c>
       <c r="E24" s="11">
@@ -1604,7 +1669,7 @@
       <c r="C25" s="8">
         <v>1</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="17">
         <v>42133</v>
       </c>
       <c r="E25" s="11">
@@ -1624,7 +1689,7 @@
       <c r="C26" s="8">
         <v>1</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="17">
         <v>42051</v>
       </c>
       <c r="E26" s="11"/>
@@ -1642,7 +1707,7 @@
       <c r="C27" s="8">
         <v>1</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="17">
         <v>41829</v>
       </c>
       <c r="E27" s="11">
@@ -1654,15 +1719,15 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>112</v>
-      </c>
       <c r="C28" s="8">
         <v>1</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="17">
         <v>41672</v>
       </c>
       <c r="E28" s="11">
@@ -1674,7 +1739,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>66</v>
@@ -1682,7 +1747,7 @@
       <c r="C29" s="8">
         <v>1</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="17">
         <v>41881</v>
       </c>
       <c r="E29" s="11">
@@ -1694,15 +1759,15 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30" s="8">
         <v>1</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="17">
         <v>41853</v>
       </c>
       <c r="E30" s="11">
@@ -1714,15 +1779,15 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>117</v>
-      </c>
       <c r="C31" s="8">
         <v>1</v>
       </c>
-      <c r="D31" s="18">
+      <c r="D31" s="17">
         <v>41867</v>
       </c>
       <c r="E31" s="11">
@@ -1734,15 +1799,15 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C32" s="8">
         <v>1</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32" s="17">
         <v>41872</v>
       </c>
       <c r="E32" s="11">
@@ -1763,7 +1828,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>73</v>
@@ -1771,7 +1836,7 @@
       <c r="C33" s="8">
         <v>1</v>
       </c>
-      <c r="D33" s="18">
+      <c r="D33" s="17">
         <v>41870</v>
       </c>
       <c r="E33" s="11">
@@ -1783,7 +1848,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>77</v>
@@ -1791,17 +1856,17 @@
       <c r="C34" s="8">
         <v>1</v>
       </c>
-      <c r="D34" s="18">
+      <c r="D34" s="17">
         <v>41963</v>
       </c>
       <c r="E34" s="11">
         <v>1</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H34" t="s">
         <v>96</v>
@@ -1812,7 +1877,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>76</v>
@@ -1820,22 +1885,22 @@
       <c r="C35" s="8">
         <v>1</v>
       </c>
-      <c r="D35" s="18">
+      <c r="D35" s="17">
         <v>41712</v>
       </c>
       <c r="E35" s="11">
         <v>1</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>74</v>
@@ -1843,53 +1908,53 @@
       <c r="C36" s="8">
         <v>2</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D36" s="17">
         <v>41880</v>
       </c>
       <c r="E36" s="11">
         <v>1</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="C37" s="8">
         <v>1</v>
       </c>
-      <c r="D37" s="18">
+      <c r="D37" s="17">
         <v>41853</v>
       </c>
       <c r="E37" s="11">
         <v>1</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C38" s="8">
         <v>1</v>
       </c>
-      <c r="D38" s="18">
+      <c r="D38" s="17">
         <v>41823</v>
       </c>
       <c r="E38" s="11">
@@ -1899,7 +1964,7 @@
         <v>60</v>
       </c>
       <c r="G38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H38" t="s">
         <v>20</v>
@@ -1910,15 +1975,15 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>135</v>
-      </c>
       <c r="C39" s="8">
         <v>1</v>
       </c>
-      <c r="D39" s="18">
+      <c r="D39" s="17">
         <v>41694</v>
       </c>
       <c r="E39" s="11">
@@ -1928,23 +1993,43 @@
         <v>60</v>
       </c>
       <c r="G39" t="s">
+        <v>144</v>
+      </c>
+      <c r="H39" t="s">
+        <v>143</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C40" s="8">
         <v>1</v>
       </c>
-      <c r="D40" s="18">
+      <c r="D40" s="17">
         <v>42073</v>
       </c>
-      <c r="E40" s="11"/>
+      <c r="E40" s="11">
+        <v>1</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G40" t="s">
+        <v>95</v>
+      </c>
+      <c r="H40" t="s">
+        <v>96</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
@@ -1956,29 +2041,42 @@
       <c r="C41" s="8">
         <v>1</v>
       </c>
-      <c r="D41" s="18">
+      <c r="D41" s="17">
         <v>41927</v>
       </c>
-      <c r="E41" s="11"/>
+      <c r="E41" s="11">
+        <v>1</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C42" s="8">
         <v>1</v>
       </c>
-      <c r="D42" s="18">
+      <c r="D42" s="17">
         <v>42146</v>
       </c>
-      <c r="E42" s="11"/>
+      <c r="E42" s="11">
+        <v>1</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G42" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>71</v>
@@ -1986,14 +2084,22 @@
       <c r="C43" s="8">
         <v>1</v>
       </c>
-      <c r="D43" s="18">
+      <c r="D43" s="17">
         <v>42111</v>
       </c>
-      <c r="E43" s="11"/>
+      <c r="E43" s="11">
+        <v>1</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G43" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>72</v>
@@ -2001,84 +2107,97 @@
       <c r="C44" s="8">
         <v>1</v>
       </c>
-      <c r="D44" s="18">
+      <c r="D44" s="17">
         <v>41888</v>
       </c>
-      <c r="E44" s="11"/>
+      <c r="E44" s="11">
+        <v>1</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E46" s="15"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
+      <c r="B46" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B50">
+      <c r="B47" s="18">
         <v>26</v>
       </c>
-      <c r="D50" s="19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B51">
-        <f>SUM(E2:E46)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="B48" s="18">
+        <f>SUM(E2:E45)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B52">
-        <f>B50-B51</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="B49" s="18">
+        <f>B47-B48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B54">
+      <c r="B51" s="18">
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B55">
+      <c r="B52" s="18">
         <f>ROWS(F2:F26)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B56">
-        <f>B54-B55</f>
+      <c r="B53" s="18">
+        <f>B51-B52</f>
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B55" s="24" t="s">
         <v>107</v>
       </c>
+      <c r="C55" s="22"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>